<commit_message>
Deixando o Processo mais Inteligente
</commit_message>
<xml_diff>
--- a/Planilha Base.xlsx
+++ b/Planilha Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Programs - Dados/Projetos/Preenche Planilhas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CCD488-3FDE-DF40-B8D2-5AB69EB63311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4258683-F37D-7740-9B5E-E732087E043B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14360" xr2:uid="{B4502988-01F8-4058-9535-8A6513F01259}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ITENS DE CONTRATAÇÃO</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Número da Meta Específica</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Destinação</t>
   </si>
 </sst>
 </file>
@@ -503,9 +509,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49176E52-7C41-4F5F-B77F-576AFDC496BE}">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -513,17 +519,16 @@
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="18.5" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="3" max="6" width="19.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -536,8 +541,10 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
-    </row>
-    <row r="2" spans="1:10" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -551,25 +558,31 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -578,10 +591,12 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -590,10 +605,12 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -602,10 +619,12 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -614,10 +633,12 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -626,10 +647,12 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -638,10 +661,12 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -650,10 +675,12 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -662,10 +689,12 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -674,10 +703,12 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -686,10 +717,12 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -698,10 +731,12 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -710,10 +745,12 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -722,10 +759,12 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -734,10 +773,12 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -746,10 +787,12 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -758,10 +801,12 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -770,10 +815,12 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -782,10 +829,12 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -794,10 +843,12 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -806,10 +857,12 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -818,10 +871,12 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -830,10 +885,12 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -842,10 +899,12 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -854,10 +913,12 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -866,10 +927,12 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -878,10 +941,12 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -890,10 +955,12 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -902,10 +969,12 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -914,10 +983,12 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="5"/>
+    </row>
+    <row r="32" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -926,10 +997,12 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="5"/>
+    </row>
+    <row r="33" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -938,10 +1011,12 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="5"/>
-    </row>
-    <row r="34" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="5"/>
+    </row>
+    <row r="34" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -950,10 +1025,12 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="5"/>
+    </row>
+    <row r="35" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -962,10 +1039,12 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="5"/>
+    </row>
+    <row r="36" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -974,10 +1053,12 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="5"/>
+    </row>
+    <row r="37" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -986,10 +1067,12 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="5"/>
+    </row>
+    <row r="38" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -998,10 +1081,12 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="5"/>
+    </row>
+    <row r="39" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1010,10 +1095,12 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="5"/>
+    </row>
+    <row r="40" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1022,10 +1109,12 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="5"/>
+    </row>
+    <row r="41" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1034,10 +1123,12 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="5"/>
+    </row>
+    <row r="42" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1046,10 +1137,12 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1058,10 +1151,12 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="5"/>
-    </row>
-    <row r="44" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="5"/>
+    </row>
+    <row r="44" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1070,10 +1165,12 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="5"/>
-    </row>
-    <row r="45" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1082,10 +1179,12 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="5"/>
+    </row>
+    <row r="46" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1094,10 +1193,12 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="5"/>
+    </row>
+    <row r="47" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1106,10 +1207,12 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="5"/>
+    </row>
+    <row r="48" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1118,10 +1221,12 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="5"/>
+    </row>
+    <row r="49" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1130,10 +1235,12 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="5"/>
-    </row>
-    <row r="50" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1142,10 +1249,12 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="5"/>
+    </row>
+    <row r="51" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1154,10 +1263,12 @@
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="5"/>
-    </row>
-    <row r="52" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="5"/>
+    </row>
+    <row r="52" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1166,10 +1277,12 @@
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="5"/>
-    </row>
-    <row r="53" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="5"/>
+    </row>
+    <row r="53" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1178,10 +1291,12 @@
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="5"/>
-    </row>
-    <row r="54" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="5"/>
+    </row>
+    <row r="54" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -1190,10 +1305,12 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="5"/>
-    </row>
-    <row r="55" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="5"/>
+    </row>
+    <row r="55" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1202,10 +1319,12 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="5"/>
-    </row>
-    <row r="56" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="5"/>
+    </row>
+    <row r="56" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -1214,10 +1333,12 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="5"/>
-    </row>
-    <row r="57" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="5"/>
+    </row>
+    <row r="57" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -1226,10 +1347,12 @@
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="5"/>
-    </row>
-    <row r="58" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="5"/>
+    </row>
+    <row r="58" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -1238,10 +1361,12 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="5"/>
-    </row>
-    <row r="59" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="5"/>
+    </row>
+    <row r="59" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -1250,10 +1375,12 @@
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="5"/>
-    </row>
-    <row r="60" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="5"/>
+    </row>
+    <row r="60" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -1262,10 +1389,12 @@
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="5"/>
-    </row>
-    <row r="61" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="5"/>
+    </row>
+    <row r="61" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -1274,10 +1403,12 @@
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="5"/>
-    </row>
-    <row r="62" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="5"/>
+    </row>
+    <row r="62" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -1286,10 +1417,12 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="5"/>
-    </row>
-    <row r="63" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="5"/>
+    </row>
+    <row r="63" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -1298,10 +1431,12 @@
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="5"/>
-    </row>
-    <row r="64" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="5"/>
+    </row>
+    <row r="64" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -1310,10 +1445,12 @@
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="5"/>
-    </row>
-    <row r="65" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="5"/>
+    </row>
+    <row r="65" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -1322,10 +1459,12 @@
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="5"/>
-    </row>
-    <row r="66" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="4"/>
+      <c r="L65" s="5"/>
+    </row>
+    <row r="66" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -1334,10 +1473,12 @@
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="5"/>
-    </row>
-    <row r="67" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="5"/>
+    </row>
+    <row r="67" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -1346,10 +1487,12 @@
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="5"/>
-    </row>
-    <row r="68" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="5"/>
+    </row>
+    <row r="68" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -1358,10 +1501,12 @@
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
-      <c r="I68" s="4"/>
-      <c r="J68" s="5"/>
-    </row>
-    <row r="69" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="5"/>
+    </row>
+    <row r="69" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -1370,10 +1515,12 @@
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
-      <c r="I69" s="4"/>
-      <c r="J69" s="5"/>
-    </row>
-    <row r="70" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="5"/>
+    </row>
+    <row r="70" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -1382,10 +1529,12 @@
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="5"/>
-    </row>
-    <row r="71" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="5"/>
+    </row>
+    <row r="71" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -1394,10 +1543,12 @@
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="5"/>
-    </row>
-    <row r="72" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="5"/>
+    </row>
+    <row r="72" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -1406,10 +1557,12 @@
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
-      <c r="I72" s="4"/>
-      <c r="J72" s="5"/>
-    </row>
-    <row r="73" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="5"/>
+    </row>
+    <row r="73" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -1418,10 +1571,12 @@
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="5"/>
-    </row>
-    <row r="74" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="5"/>
+    </row>
+    <row r="74" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -1430,10 +1585,12 @@
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="5"/>
-    </row>
-    <row r="75" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="4"/>
+      <c r="L74" s="5"/>
+    </row>
+    <row r="75" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -1442,10 +1599,12 @@
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="5"/>
-    </row>
-    <row r="76" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="4"/>
+      <c r="L75" s="5"/>
+    </row>
+    <row r="76" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -1454,10 +1613,12 @@
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
-      <c r="I76" s="4"/>
-      <c r="J76" s="5"/>
-    </row>
-    <row r="77" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="4"/>
+      <c r="L76" s="5"/>
+    </row>
+    <row r="77" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -1466,10 +1627,12 @@
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
-      <c r="I77" s="4"/>
-      <c r="J77" s="5"/>
-    </row>
-    <row r="78" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="5"/>
+    </row>
+    <row r="78" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -1478,10 +1641,12 @@
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="5"/>
-    </row>
-    <row r="79" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="4"/>
+      <c r="L78" s="5"/>
+    </row>
+    <row r="79" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -1490,10 +1655,12 @@
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="5"/>
-    </row>
-    <row r="80" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="4"/>
+      <c r="L79" s="5"/>
+    </row>
+    <row r="80" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -1502,10 +1669,12 @@
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="5"/>
-    </row>
-    <row r="81" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="5"/>
+    </row>
+    <row r="81" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -1514,10 +1683,12 @@
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="5"/>
-    </row>
-    <row r="82" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="4"/>
+      <c r="L81" s="5"/>
+    </row>
+    <row r="82" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -1526,10 +1697,12 @@
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="5"/>
-    </row>
-    <row r="83" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="4"/>
+      <c r="L82" s="5"/>
+    </row>
+    <row r="83" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -1538,10 +1711,12 @@
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="5"/>
-    </row>
-    <row r="84" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="4"/>
+      <c r="L83" s="5"/>
+    </row>
+    <row r="84" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -1550,10 +1725,12 @@
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="5"/>
-    </row>
-    <row r="85" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="5"/>
+    </row>
+    <row r="85" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -1562,10 +1739,12 @@
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="5"/>
-    </row>
-    <row r="86" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="4"/>
+      <c r="L85" s="5"/>
+    </row>
+    <row r="86" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -1574,10 +1753,12 @@
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="5"/>
-    </row>
-    <row r="87" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="5"/>
+    </row>
+    <row r="87" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -1586,10 +1767,12 @@
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
-      <c r="I87" s="4"/>
-      <c r="J87" s="5"/>
-    </row>
-    <row r="88" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I87" s="3"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="4"/>
+      <c r="L87" s="5"/>
+    </row>
+    <row r="88" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -1598,10 +1781,12 @@
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
-      <c r="I88" s="4"/>
-      <c r="J88" s="5"/>
-    </row>
-    <row r="89" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="5"/>
+    </row>
+    <row r="89" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -1610,10 +1795,12 @@
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
-      <c r="I89" s="4"/>
-      <c r="J89" s="5"/>
-    </row>
-    <row r="90" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="5"/>
+    </row>
+    <row r="90" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -1622,10 +1809,12 @@
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
-      <c r="I90" s="4"/>
-      <c r="J90" s="5"/>
-    </row>
-    <row r="91" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="5"/>
+    </row>
+    <row r="91" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -1634,10 +1823,12 @@
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
-      <c r="I91" s="4"/>
-      <c r="J91" s="5"/>
-    </row>
-    <row r="92" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="4"/>
+      <c r="L91" s="5"/>
+    </row>
+    <row r="92" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -1646,10 +1837,12 @@
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
-      <c r="I92" s="4"/>
-      <c r="J92" s="5"/>
-    </row>
-    <row r="93" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="5"/>
+    </row>
+    <row r="93" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -1658,10 +1851,12 @@
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
-      <c r="I93" s="4"/>
-      <c r="J93" s="5"/>
-    </row>
-    <row r="94" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I93" s="3"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="4"/>
+      <c r="L93" s="5"/>
+    </row>
+    <row r="94" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -1670,10 +1865,12 @@
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
-      <c r="I94" s="4"/>
-      <c r="J94" s="5"/>
-    </row>
-    <row r="95" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="4"/>
+      <c r="L94" s="5"/>
+    </row>
+    <row r="95" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -1682,10 +1879,12 @@
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
-      <c r="I95" s="4"/>
-      <c r="J95" s="5"/>
-    </row>
-    <row r="96" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="5"/>
+    </row>
+    <row r="96" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -1694,10 +1893,12 @@
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
-      <c r="I96" s="4"/>
-      <c r="J96" s="5"/>
-    </row>
-    <row r="97" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="4"/>
+      <c r="L96" s="5"/>
+    </row>
+    <row r="97" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -1706,10 +1907,12 @@
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
-      <c r="I97" s="4"/>
-      <c r="J97" s="5"/>
-    </row>
-    <row r="98" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I97" s="3"/>
+      <c r="J97" s="3"/>
+      <c r="K97" s="4"/>
+      <c r="L97" s="5"/>
+    </row>
+    <row r="98" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -1718,10 +1921,12 @@
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
-      <c r="I98" s="4"/>
-      <c r="J98" s="5"/>
-    </row>
-    <row r="99" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I98" s="3"/>
+      <c r="J98" s="3"/>
+      <c r="K98" s="4"/>
+      <c r="L98" s="5"/>
+    </row>
+    <row r="99" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -1730,10 +1935,12 @@
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
-      <c r="I99" s="4"/>
-      <c r="J99" s="5"/>
-    </row>
-    <row r="100" spans="1:10" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I99" s="3"/>
+      <c r="J99" s="3"/>
+      <c r="K99" s="4"/>
+      <c r="L99" s="5"/>
+    </row>
+    <row r="100" spans="1:12" ht="222" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -1742,13 +1949,15 @@
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
-      <c r="I100" s="4"/>
-      <c r="J100" s="5"/>
-    </row>
-    <row r="101" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="I100" s="3"/>
+      <c r="J100" s="3"/>
+      <c r="K100" s="4"/>
+      <c r="L100" s="5"/>
+    </row>
+    <row r="101" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Att no scrool e no zoom da planilha
</commit_message>
<xml_diff>
--- a/Planilha Base.xlsx
+++ b/Planilha Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Programs - Dados/Projetos/Preenche Planilhas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C561982-01B1-C749-82B3-076276096220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FADCEC1-87AF-5C43-A165-6484C46EBA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14360" xr2:uid="{B4502988-01F8-4058-9535-8A6513F01259}"/>
   </bookViews>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49176E52-7C41-4F5F-B77F-576AFDC496BE}">
   <dimension ref="A1:L3288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3138" zoomScale="43" zoomScaleNormal="43" workbookViewId="0">
-      <selection activeCell="O3141" sqref="O3141"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Sanitiza template e remove planilhas de teste
</commit_message>
<xml_diff>
--- a/Planilha Base.xlsx
+++ b/Planilha Base.xlsx
@@ -706,7 +706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:L137"/>
+  <dimension ref="A1:L137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H25" sqref="E6:J35"/>
@@ -797,11 +797,7 @@
           <t>SIM, conforme elementos analisados no Plano de Aplicação.</t>
         </is>
       </c>
-      <c r="F4" s="9" t="inlineStr">
-        <is>
-          <t>SIM, pois está entre as metas do PNSP, bem como no enfoque desta Área Temática.</t>
-        </is>
-      </c>
+      <c r="F4" s="9" t="inlineStr"/>
       <c r="G4" s="12" t="n"/>
       <c r="H4" s="12" t="n"/>
       <c r="I4" s="12" t="n"/>
@@ -898,32 +894,32 @@
     <row r="8" ht="148.5" customHeight="1" thickBot="1" thickTop="1">
       <c r="A8" s="9" t="inlineStr">
         <is>
-          <t>1* Redução da taxa estadual de Morte Violenta Intencional para no máximo de 6,41 por 100 mil habitantes até 2027. A taxa atual é de 8,41 mortes por grupo de 100 mil habitantes em 2024, segundo dados do SINESP.1*</t>
+          <t>1*1*</t>
         </is>
       </c>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>SIM, pois foi estabelecida uma meta geral que reflete o problema público e demonstrada uma estratégia adequada para a sua mitigação.</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="C8" s="9" t="inlineStr">
         <is>
-          <t>SIM, pois houve a identificação de um relevante problema público selecionado como objeto da intervenção proposta, bem como um indicador capaz de demonstrar a implementação.</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="D8" s="9" t="inlineStr">
         <is>
-          <t>SIM, pois verifica-se a relação direta entre as medidas propostas e a meta geral estabelecida.</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="E8" s="9" t="inlineStr">
         <is>
-          <t>SIM, já que foram indicadas ações que em conjunto permitem o atingimento das metas específicas e, consequentemente da meta geral.</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="F8" s="9" t="inlineStr">
         <is>
-          <t>SIM, o indicador é capaz de mensurar o desempenho dos processos voltados ao atingimento da Meta geral.</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="G8" s="12" t="n"/>
@@ -959,7 +955,7 @@
       <c r="E10" s="11" t="n"/>
       <c r="F10" s="9" t="inlineStr">
         <is>
-          <t>0* Indicador: Taxa de mortes violentas Finalidade: Verificar a variação da taxa de mortes violentas Fórmula de cálculo: (Σ de vítimas homicídio doloso + feminicídio + latrocínio + lesão corporal seguida de morte + morte por intervenção policial x 100 mil) /população Periodicidade: Anual Índice Atual de SC 2025: 8,41% (SINESP) Variação (atual/meta): -52,5% Meta 2030 Plano Estadual: 6,0 Fonte: Plano Estadual de Segurança Pública e Defesa Social II de Santa Catarina.0*</t>
+          <t>0*0*</t>
         </is>
       </c>
       <c r="G10" s="12" t="n"/>
@@ -1007,22 +1003,22 @@
       <c r="A12" s="11" t="n"/>
       <c r="B12" s="9" t="inlineStr">
         <is>
-          <t>ATENDE, pois identifica e delimita o problema público a ser enfrentado.</t>
+          <t>ATENDE.</t>
         </is>
       </c>
       <c r="C12" s="9" t="inlineStr">
         <is>
-          <t>ATENDE e aponta os referidos mecanismos adequadamente.</t>
+          <t>ATENDE.</t>
         </is>
       </c>
       <c r="D12" s="9" t="inlineStr">
         <is>
-          <t>ATENDE, pois houve demonstração da pretensão de difundir os conhecimentos do tema aos policiais que atuam na área, além disso foi demonstrada a intenção de efetivar uma atuação integrada.</t>
+          <t>ATENDE.</t>
         </is>
       </c>
       <c r="E12" s="9" t="inlineStr">
         <is>
-          <t>ATENDE, pois foram indicadas contratações de objetos e serviços com o objetivo de mitigar o déficit de equipamentos, aumentar a capacidade de prestação dos serviços no intuito de implementar a Meta Geral estabelecida no Plano de Aplicação.</t>
+          <t>ATENDE.</t>
         </is>
       </c>
       <c r="F12" s="12" t="n"/>
@@ -1066,17 +1062,17 @@
       </c>
       <c r="G13" s="20" t="inlineStr">
         <is>
-          <t>A Meta do PESP foi informada? Existe aderência?</t>
+          <t>A Meta setorial foi informada? Existe aderência?</t>
         </is>
       </c>
       <c r="H13" s="20" t="inlineStr">
         <is>
-          <t>A Meta do PNSP foi informada? Existe aderência?</t>
+          <t>A Meta nacional foi informada? Existe aderência?</t>
         </is>
       </c>
       <c r="I13" s="20" t="inlineStr">
         <is>
-          <t>A política da Carteira de Políticas do MJSP foi informada? Existe aderência?</t>
+          <t>A política informada foi apresentada? Existe aderência?</t>
         </is>
       </c>
       <c r="J13" s="12" t="n"/>
@@ -1086,7 +1082,7 @@
     <row r="14" ht="17" customHeight="1" thickBot="1" thickTop="1">
       <c r="A14" s="21" t="inlineStr">
         <is>
-          <t>2*1 - Reduzir em 20% a taxa de homicídios e feminicídios, latrocínios e lesões corporais seguida de morte nos 60 municípios com população igual ou superior a 26.500 habitantes até 2027.2*</t>
+          <t>2*2*</t>
         </is>
       </c>
       <c r="B14" s="9" t="inlineStr">
@@ -1108,8 +1104,7 @@
         <is>
           <t>SIM.
 A referência informada foi:
-3*Referência: 371 homicídios/feminicídios, 
-29 lesões corporais seguidas de morte e 16 latrocínios = 416 registros - GEAC/DINE/SSP/SC - 2024.3*</t>
+3*3*</t>
         </is>
       </c>
       <c r="F14" s="9" t="inlineStr">
@@ -1117,9 +1112,9 @@
           <t>SIM.
 O Indicador e Fórmula de Cálculo informado foi:
 4*Descrição do Indicador:
-Taxa(%) de ocorrências atendidas.4*
+4*
 5*Fórmula:
-(Nº de ocorrências atendidas após a aquisição*100 / Nº de ocorrências atendidas realizadasantes da aquisção) - 100.5*
+5*
 O indicador e a fórmula de cálculo são adequados para o eficiente monitoramento da meta.</t>
         </is>
       </c>
@@ -1127,7 +1122,7 @@
         <is>
           <t>SIM.
 A Meta informada foi:
-6*1ª Diretriz: Enfrentamento a criminalidade violenta. Ações Estratégicas 1. Redução dos homicídios. Taxa igual ou menor que 6,0/100 mil/hab. até 2030.6*
+6*6*
 Existe aderência da referida Meta à Política Pública.</t>
         </is>
       </c>
@@ -1135,7 +1130,7 @@
         <is>
           <t>SIM.
 A Meta informada foi:
-7*Meta 1: Reduzir a taxa nacional de homicídios para abaixo de 16 mortes por 100 mil habitantes até 2030.7*
+7*7*
 Existe aderência da referida Meta Específica à Política informada.</t>
         </is>
       </c>
@@ -1143,7 +1138,7 @@
         <is>
           <t>SIM.
 A política informada foi:
-8*Política de Enfrentamento da Criminalidade Violenta.8*
+8*8*
 Existe aderência da referida Meta Específica à Política informada.</t>
         </is>
       </c>
@@ -1274,15 +1269,68 @@
       <c r="L24" s="19" t="n"/>
     </row>
     <row r="25" ht="19.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A25" s="14" t="n"/>
-      <c r="B25" s="9" t="n"/>
-      <c r="C25" s="9" t="n"/>
-      <c r="D25" s="9" t="n"/>
-      <c r="E25" s="9" t="n"/>
-      <c r="F25" s="9" t="n"/>
-      <c r="G25" s="9" t="n"/>
-      <c r="H25" s="9" t="n"/>
-      <c r="I25" s="9" t="n"/>
+      <c r="A25" s="14" t="inlineStr">
+        <is>
+          <t>2*2*</t>
+        </is>
+      </c>
+      <c r="B25" s="9" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="C25" s="9" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="D25" s="9" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="E25" s="9" t="inlineStr">
+        <is>
+          <t>SIM.
+A referência informada foi:
+3*3*</t>
+        </is>
+      </c>
+      <c r="F25" s="9" t="inlineStr">
+        <is>
+          <t>SIM.
+O Indicador e Fórmula de Cálculo informado foi:
+4*Descrição do Indicador:
+4*
+5*Fórmula:
+5*
+O indicador e a fórmula de cálculo são adequados para o eficiente monitoramento da meta.</t>
+        </is>
+      </c>
+      <c r="G25" s="9" t="inlineStr">
+        <is>
+          <t>SIM.
+A Meta informada foi:
+6*6*
+Existe aderência da referida Meta à Política Pública.</t>
+        </is>
+      </c>
+      <c r="H25" s="9" t="inlineStr">
+        <is>
+          <t>SIM.
+A Meta informada foi:
+7*7*
+Existe aderência da referida Meta Específica à Política informada.</t>
+        </is>
+      </c>
+      <c r="I25" s="9" t="inlineStr">
+        <is>
+          <t>SIM.
+A política informada foi:
+8*8*
+Existe aderência da referida Meta Específica à Política informada.</t>
+        </is>
+      </c>
       <c r="J25" s="26" t="n"/>
       <c r="K25" s="26" t="n"/>
       <c r="L25" s="15" t="n"/>
@@ -2881,8 +2929,8 @@
     <mergeCell ref="F4:L4"/>
     <mergeCell ref="D25:D35"/>
     <mergeCell ref="A14:A24"/>
+    <mergeCell ref="F10:L10"/>
     <mergeCell ref="G14:G24"/>
-    <mergeCell ref="F10:L10"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A38:L38"/>

</xml_diff>

<commit_message>
Restaura conteudo completo da Planilha Base
</commit_message>
<xml_diff>
--- a/Planilha Base.xlsx
+++ b/Planilha Base.xlsx
@@ -706,7 +706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L137"/>
+  <dimension ref="A2:L137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H25" sqref="E6:J35"/>
@@ -797,7 +797,11 @@
           <t>SIM, conforme elementos analisados no Plano de Aplicação.</t>
         </is>
       </c>
-      <c r="F4" s="9" t="inlineStr"/>
+      <c r="F4" s="9" t="inlineStr">
+        <is>
+          <t>SIM, pois está entre as metas do PNSP, bem como no enfoque desta Área Temática.</t>
+        </is>
+      </c>
       <c r="G4" s="12" t="n"/>
       <c r="H4" s="12" t="n"/>
       <c r="I4" s="12" t="n"/>
@@ -894,32 +898,32 @@
     <row r="8" ht="148.5" customHeight="1" thickBot="1" thickTop="1">
       <c r="A8" s="9" t="inlineStr">
         <is>
-          <t>1*1*</t>
+          <t>1* Redução da taxa estadual de Morte Violenta Intencional para no máximo de 6,41 por 100 mil habitantes até 2027. A taxa atual é de 8,41 mortes por grupo de 100 mil habitantes em 2024, segundo dados do SINESP.1*</t>
         </is>
       </c>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>SIM, pois foi estabelecida uma meta geral que reflete o problema público e demonstrada uma estratégia adequada para a sua mitigação.</t>
         </is>
       </c>
       <c r="C8" s="9" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>SIM, pois houve a identificação de um relevante problema público selecionado como objeto da intervenção proposta, bem como um indicador capaz de demonstrar a implementação.</t>
         </is>
       </c>
       <c r="D8" s="9" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>SIM, pois verifica-se a relação direta entre as medidas propostas e a meta geral estabelecida.</t>
         </is>
       </c>
       <c r="E8" s="9" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>SIM, já que foram indicadas ações que em conjunto permitem o atingimento das metas específicas e, consequentemente da meta geral.</t>
         </is>
       </c>
       <c r="F8" s="9" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>SIM, o indicador é capaz de mensurar o desempenho dos processos voltados ao atingimento da Meta geral.</t>
         </is>
       </c>
       <c r="G8" s="12" t="n"/>
@@ -955,7 +959,7 @@
       <c r="E10" s="11" t="n"/>
       <c r="F10" s="9" t="inlineStr">
         <is>
-          <t>0*0*</t>
+          <t>0* Indicador: Taxa de mortes violentas Finalidade: Verificar a variação da taxa de mortes violentas Fórmula de cálculo: (Σ de vítimas homicídio doloso + feminicídio + latrocínio + lesão corporal seguida de morte + morte por intervenção policial x 100 mil) /população Periodicidade: Anual Índice Atual de SC 2025: 8,41% (SINESP) Variação (atual/meta): -52,5% Meta 2030 Plano Estadual: 6,0 Fonte: Plano Estadual de Segurança Pública e Defesa Social II de Santa Catarina.0*</t>
         </is>
       </c>
       <c r="G10" s="12" t="n"/>
@@ -1003,22 +1007,22 @@
       <c r="A12" s="11" t="n"/>
       <c r="B12" s="9" t="inlineStr">
         <is>
-          <t>ATENDE.</t>
+          <t>ATENDE, pois identifica e delimita o problema público a ser enfrentado.</t>
         </is>
       </c>
       <c r="C12" s="9" t="inlineStr">
         <is>
-          <t>ATENDE.</t>
+          <t>ATENDE e aponta os referidos mecanismos adequadamente.</t>
         </is>
       </c>
       <c r="D12" s="9" t="inlineStr">
         <is>
-          <t>ATENDE.</t>
+          <t>ATENDE, pois houve demonstração da pretensão de difundir os conhecimentos do tema aos policiais que atuam na área, além disso foi demonstrada a intenção de efetivar uma atuação integrada.</t>
         </is>
       </c>
       <c r="E12" s="9" t="inlineStr">
         <is>
-          <t>ATENDE.</t>
+          <t>ATENDE, pois foram indicadas contratações de objetos e serviços com o objetivo de mitigar o déficit de equipamentos, aumentar a capacidade de prestação dos serviços no intuito de implementar a Meta Geral estabelecida no Plano de Aplicação.</t>
         </is>
       </c>
       <c r="F12" s="12" t="n"/>
@@ -1062,17 +1066,17 @@
       </c>
       <c r="G13" s="20" t="inlineStr">
         <is>
-          <t>A Meta setorial foi informada? Existe aderência?</t>
+          <t>A Meta do PESP foi informada? Existe aderência?</t>
         </is>
       </c>
       <c r="H13" s="20" t="inlineStr">
         <is>
-          <t>A Meta nacional foi informada? Existe aderência?</t>
+          <t>A Meta do PNSP foi informada? Existe aderência?</t>
         </is>
       </c>
       <c r="I13" s="20" t="inlineStr">
         <is>
-          <t>A política informada foi apresentada? Existe aderência?</t>
+          <t>A política da Carteira de Políticas do MJSP foi informada? Existe aderência?</t>
         </is>
       </c>
       <c r="J13" s="12" t="n"/>
@@ -1082,7 +1086,7 @@
     <row r="14" ht="17" customHeight="1" thickBot="1" thickTop="1">
       <c r="A14" s="21" t="inlineStr">
         <is>
-          <t>2*2*</t>
+          <t>2*1 - Reduzir em 20% a taxa de homicídios e feminicídios, latrocínios e lesões corporais seguida de morte nos 60 municípios com população igual ou superior a 26.500 habitantes até 2027.2*</t>
         </is>
       </c>
       <c r="B14" s="9" t="inlineStr">
@@ -1104,7 +1108,8 @@
         <is>
           <t>SIM.
 A referência informada foi:
-3*3*</t>
+3*Referência: 371 homicídios/feminicídios, 
+29 lesões corporais seguidas de morte e 16 latrocínios = 416 registros - GEAC/DINE/SSP/SC - 2024.3*</t>
         </is>
       </c>
       <c r="F14" s="9" t="inlineStr">
@@ -1112,9 +1117,9 @@
           <t>SIM.
 O Indicador e Fórmula de Cálculo informado foi:
 4*Descrição do Indicador:
-4*
+Taxa(%) de ocorrências atendidas.4*
 5*Fórmula:
-5*
+(Nº de ocorrências atendidas após a aquisição*100 / Nº de ocorrências atendidas realizadasantes da aquisção) - 100.5*
 O indicador e a fórmula de cálculo são adequados para o eficiente monitoramento da meta.</t>
         </is>
       </c>
@@ -1122,7 +1127,7 @@
         <is>
           <t>SIM.
 A Meta informada foi:
-6*6*
+6*1ª Diretriz: Enfrentamento a criminalidade violenta. Ações Estratégicas 1. Redução dos homicídios. Taxa igual ou menor que 6,0/100 mil/hab. até 2030.6*
 Existe aderência da referida Meta à Política Pública.</t>
         </is>
       </c>
@@ -1130,7 +1135,7 @@
         <is>
           <t>SIM.
 A Meta informada foi:
-7*7*
+7*Meta 1: Reduzir a taxa nacional de homicídios para abaixo de 16 mortes por 100 mil habitantes até 2030.7*
 Existe aderência da referida Meta Específica à Política informada.</t>
         </is>
       </c>
@@ -1138,7 +1143,7 @@
         <is>
           <t>SIM.
 A política informada foi:
-8*8*
+8*Política de Enfrentamento da Criminalidade Violenta.8*
 Existe aderência da referida Meta Específica à Política informada.</t>
         </is>
       </c>
@@ -1269,68 +1274,15 @@
       <c r="L24" s="19" t="n"/>
     </row>
     <row r="25" ht="19.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A25" s="14" t="inlineStr">
-        <is>
-          <t>2*2*</t>
-        </is>
-      </c>
-      <c r="B25" s="9" t="inlineStr">
-        <is>
-          <t>SIM</t>
-        </is>
-      </c>
-      <c r="C25" s="9" t="inlineStr">
-        <is>
-          <t>SIM</t>
-        </is>
-      </c>
-      <c r="D25" s="9" t="inlineStr">
-        <is>
-          <t>SIM</t>
-        </is>
-      </c>
-      <c r="E25" s="9" t="inlineStr">
-        <is>
-          <t>SIM.
-A referência informada foi:
-3*3*</t>
-        </is>
-      </c>
-      <c r="F25" s="9" t="inlineStr">
-        <is>
-          <t>SIM.
-O Indicador e Fórmula de Cálculo informado foi:
-4*Descrição do Indicador:
-4*
-5*Fórmula:
-5*
-O indicador e a fórmula de cálculo são adequados para o eficiente monitoramento da meta.</t>
-        </is>
-      </c>
-      <c r="G25" s="9" t="inlineStr">
-        <is>
-          <t>SIM.
-A Meta informada foi:
-6*6*
-Existe aderência da referida Meta à Política Pública.</t>
-        </is>
-      </c>
-      <c r="H25" s="9" t="inlineStr">
-        <is>
-          <t>SIM.
-A Meta informada foi:
-7*7*
-Existe aderência da referida Meta Específica à Política informada.</t>
-        </is>
-      </c>
-      <c r="I25" s="9" t="inlineStr">
-        <is>
-          <t>SIM.
-A política informada foi:
-8*8*
-Existe aderência da referida Meta Específica à Política informada.</t>
-        </is>
-      </c>
+      <c r="A25" s="14" t="n"/>
+      <c r="B25" s="9" t="n"/>
+      <c r="C25" s="9" t="n"/>
+      <c r="D25" s="9" t="n"/>
+      <c r="E25" s="9" t="n"/>
+      <c r="F25" s="9" t="n"/>
+      <c r="G25" s="9" t="n"/>
+      <c r="H25" s="9" t="n"/>
+      <c r="I25" s="9" t="n"/>
       <c r="J25" s="26" t="n"/>
       <c r="K25" s="26" t="n"/>
       <c r="L25" s="15" t="n"/>
@@ -2929,8 +2881,8 @@
     <mergeCell ref="F4:L4"/>
     <mergeCell ref="D25:D35"/>
     <mergeCell ref="A14:A24"/>
+    <mergeCell ref="G14:G24"/>
     <mergeCell ref="F10:L10"/>
-    <mergeCell ref="G14:G24"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A38:L38"/>

</xml_diff>